<commit_message>
New data and Add gitignore
</commit_message>
<xml_diff>
--- a/更版 (3).xlsx
+++ b/更版 (3).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesse/Documents/NCKU/112-2/Patrick/data-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCFA08F-82AC-884A-BC08-0A7E200E7281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7745C63D-0C7A-9E44-B77A-EC5144097198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="19340" xr2:uid="{05084C73-5F64-4147-B5B8-CCFB290F5584}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16800" windowHeight="19340" xr2:uid="{05084C73-5F64-4147-B5B8-CCFB290F5584}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表4" sheetId="4" r:id="rId1"/>
@@ -1435,10 +1435,10 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD19"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1"/>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="26" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A26" s="4" t="s">
         <v>81</v>
       </c>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="27" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A27" s="4" t="s">
         <v>101</v>
       </c>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="28" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A28" s="27" t="s">
         <v>103</v>
       </c>
@@ -1962,7 +1962,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="29" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A29" s="27" t="s">
         <v>104</v>
       </c>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="30" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A30" s="27" t="s">
         <v>104</v>
       </c>
@@ -2000,7 +2000,7 @@
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="31" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A31" s="4" t="s">
         <v>11</v>
       </c>
@@ -2019,7 +2019,7 @@
       </c>
       <c r="G31" s="11"/>
     </row>
-    <row r="32" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="32" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A32" s="22" t="s">
         <v>30</v>
       </c>
@@ -2040,7 +2040,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="33" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A33" s="4" t="s">
         <v>20</v>
       </c>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="34" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A34" s="22" t="s">
         <v>24</v>
       </c>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="35" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A35" s="22" t="s">
         <v>32</v>
       </c>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="36" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A36" s="25" t="s">
         <v>64</v>
       </c>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="37" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A37" s="8" t="s">
         <v>66</v>
       </c>
@@ -2135,7 +2135,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="38" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A38" s="25" t="s">
         <v>67</v>
       </c>
@@ -2154,7 +2154,7 @@
       </c>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="39" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A39" s="4" t="s">
         <v>68</v>
       </c>
@@ -2173,7 +2173,7 @@
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="40" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A40" s="8" t="s">
         <v>71</v>
       </c>
@@ -2192,7 +2192,7 @@
       </c>
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="41" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A41" s="4" t="s">
         <v>73</v>
       </c>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="G41" s="7"/>
     </row>
-    <row r="42" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="42" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A42" s="4" t="s">
         <v>74</v>
       </c>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="48" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A48" s="23" t="s">
         <v>42</v>
       </c>
@@ -2342,7 +2342,7 @@
       </c>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="49" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A49" s="8" t="s">
         <v>43</v>
       </c>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="G49" s="7"/>
     </row>
-    <row r="50" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="50" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A50" s="8" t="s">
         <v>44</v>
       </c>
@@ -2376,7 +2376,7 @@
       </c>
       <c r="G50" s="7"/>
     </row>
-    <row r="51" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="51" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A51" s="8" t="s">
         <v>45</v>
       </c>
@@ -2393,7 +2393,7 @@
       </c>
       <c r="G51" s="11"/>
     </row>
-    <row r="52" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="52" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A52" s="18" t="s">
         <v>46</v>
       </c>
@@ -2410,7 +2410,7 @@
       </c>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="53" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A53" s="8" t="s">
         <v>47</v>
       </c>
@@ -2427,7 +2427,7 @@
       </c>
       <c r="G53" s="7"/>
     </row>
-    <row r="54" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="54" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A54" s="18" t="s">
         <v>48</v>
       </c>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="G54" s="11"/>
     </row>
-    <row r="55" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="55" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A55" s="19" t="s">
         <v>49</v>
       </c>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="G55" s="7"/>
     </row>
-    <row r="56" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="56" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A56" s="4" t="s">
         <v>50</v>
       </c>
@@ -2478,7 +2478,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="57" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A57" s="19" t="s">
         <v>51</v>
       </c>
@@ -2495,7 +2495,7 @@
       </c>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="58" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A58" s="18" t="s">
         <v>52</v>
       </c>
@@ -2512,7 +2512,7 @@
       </c>
       <c r="G58" s="11"/>
     </row>
-    <row r="59" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="59" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A59" s="20" t="s">
         <v>53</v>
       </c>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="G59" s="7"/>
     </row>
-    <row r="60" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="60" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A60" s="4" t="s">
         <v>54</v>
       </c>
@@ -2546,7 +2546,7 @@
       </c>
       <c r="G60" s="11"/>
     </row>
-    <row r="61" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="61" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A61" s="8" t="s">
         <v>55</v>
       </c>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="G61" s="7"/>
     </row>
-    <row r="62" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="62" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A62" s="4" t="s">
         <v>56</v>
       </c>
@@ -2580,7 +2580,7 @@
       </c>
       <c r="G62" s="7"/>
     </row>
-    <row r="63" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="63" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A63" s="4" t="s">
         <v>57</v>
       </c>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="64" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A64" s="8" t="s">
         <v>58</v>
       </c>
@@ -2614,7 +2614,7 @@
       </c>
       <c r="G64" s="11"/>
     </row>
-    <row r="65" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="65" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A65" s="4" t="s">
         <v>59</v>
       </c>
@@ -2633,7 +2633,7 @@
       </c>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="66" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A66" s="8" t="s">
         <v>60</v>
       </c>
@@ -2650,7 +2650,7 @@
       </c>
       <c r="G66" s="11"/>
     </row>
-    <row r="67" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="67" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A67" s="4" t="s">
         <v>61</v>
       </c>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="G67" s="7"/>
     </row>
-    <row r="68" spans="1:7" s="3" customFormat="1" ht="20" customHeight="1">
+    <row r="68" spans="1:7" s="3" customFormat="1" ht="20" hidden="1" customHeight="1">
       <c r="A68" s="8" t="s">
         <v>62</v>
       </c>

</xml_diff>